<commit_message>
popravil osnovne tabelce in njihov uvoz
</commit_message>
<xml_diff>
--- a/podatki/Tabele.xlsx
+++ b/podatki/Tabele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b659fc1f114388/Dokumenti/Faks/letnik_3/OPB-projekt-UP/podatki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{2D52C8F6-3900-D84C-8B86-B81D3276F733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{797707BE-A36F-496E-AFAE-2BCCA2A642A5}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{2D52C8F6-3900-D84C-8B86-B81D3276F733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEEFA90-2841-4521-A34D-A010C8364224}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{955B8738-57D6-3842-8478-390080B00E64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955B8738-57D6-3842-8478-390080B00E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,153 +38,6 @@
     <t>TRR</t>
   </si>
   <si>
-    <t>AL11 0348 5386 HUW0 DMI2 VXP5 HXMP</t>
-  </si>
-  <si>
-    <t>MK35 709M QNVZ IS7Q V16</t>
-  </si>
-  <si>
-    <t>SE75 2208 4472 8644 0572 0873</t>
-  </si>
-  <si>
-    <t>BA04 5947 1850 7523 4577</t>
-  </si>
-  <si>
-    <t>FR26 1982 7817 18MF YWRC WRTQ 195</t>
-  </si>
-  <si>
-    <t>GI14 KYSQ YLM2 ELKW P2TR HLR</t>
-  </si>
-  <si>
-    <t>VG06 IUHD 6646 0139 6924 0484</t>
-  </si>
-  <si>
-    <t>SI72 2597 1563 8071 812</t>
-  </si>
-  <si>
-    <t>GR44 5090 716I EBNV 6CDR UJSW SKF</t>
-  </si>
-  <si>
-    <t>MR11 3678 9545 3299 2571 8044 330</t>
-  </si>
-  <si>
-    <t>FR51 0327 2429 55B4 YBSI 39DB H74</t>
-  </si>
-  <si>
-    <t>TR04 7944 4XIF I80C IDHU OTCH PK</t>
-  </si>
-  <si>
-    <t>MD05 I5NN QMUY YBAV N2PI W7CH</t>
-  </si>
-  <si>
-    <t>LI06 6198 037T CHNY 7D0O D</t>
-  </si>
-  <si>
-    <t>MT63 XPMD 5828 4SRH G0T7 WIVE OEB6 OFO</t>
-  </si>
-  <si>
-    <t>FR75 7218 1398 93ML KN0N SKYM G25</t>
-  </si>
-  <si>
-    <t>DO49 EEEY 9279 7131 2039 4172 5343</t>
-  </si>
-  <si>
-    <t>DO74 KMXS 2736 3374 7051 2887 7821</t>
-  </si>
-  <si>
-    <t>FR46 8838 0143 56FV 6L6M XHBD Q62</t>
-  </si>
-  <si>
-    <t>PT06 2688 1490 3899 0228 4428 3</t>
-  </si>
-  <si>
-    <t>CY30 8453 2401 2X1W KZZR BYWU XSYB</t>
-  </si>
-  <si>
-    <t>GB16 RGMT 4636 4935 0483 94</t>
-  </si>
-  <si>
-    <t>FR33 4988 0650 09US QDFC NKBP 428</t>
-  </si>
-  <si>
-    <t>GB31 TQMH 8275 0367 7232 56</t>
-  </si>
-  <si>
-    <t>MC62 1671 4163 88ZK K8XY WGPB R61</t>
-  </si>
-  <si>
-    <t>FR47 1144 5062 425M 0WD9 GJMT 437</t>
-  </si>
-  <si>
-    <t>NL75 JLMU 1276 5021 57</t>
-  </si>
-  <si>
-    <t>MU61 GZXH 2930 7788 9110 1073 602V LT</t>
-  </si>
-  <si>
-    <t>AD53 4891 9118 GOLQ 3I8P NCKH</t>
-  </si>
-  <si>
-    <t>FR30 7530 1424 62FO YG2B 9IUM F92</t>
-  </si>
-  <si>
-    <t>HU49 0375 4535 1745 5483 8264 7885</t>
-  </si>
-  <si>
-    <t>DK78 4952 5098 4823 14</t>
-  </si>
-  <si>
-    <t>AE84 5271 2180 1021 4992 441</t>
-  </si>
-  <si>
-    <t>LU45 207N 2NLE 2POJ TIDG</t>
-  </si>
-  <si>
-    <t>SK06 2845 2772 9231 5102 0108</t>
-  </si>
-  <si>
-    <t>IT35 Z690 5653 265S W8AO EBB0 XHO</t>
-  </si>
-  <si>
-    <t>HR70 2128 8144 3889 6147 4</t>
-  </si>
-  <si>
-    <t>FR07 3665 0521 61XT LIMX BIMQ E82</t>
-  </si>
-  <si>
-    <t>FR85 2277 1116 54GS 4BT7 YPYS X77</t>
-  </si>
-  <si>
-    <t>FR64 3334 5487 92IZ LD4A 6QAM S70</t>
-  </si>
-  <si>
-    <t>FO59 1461 0406 0435 32</t>
-  </si>
-  <si>
-    <t>RS81 5563 1050 0797 7972 08</t>
-  </si>
-  <si>
-    <t>HU97 9109 5682 7220 5208 2275 1493</t>
-  </si>
-  <si>
-    <t>CR65 0649 5945 6851 6482 3</t>
-  </si>
-  <si>
-    <t>SM35 I699 2811 455I WKRD 4JTG KA1</t>
-  </si>
-  <si>
-    <t>MT86 XVMS 6776 5VNP 51SR VU1T 1VOZ CS8</t>
-  </si>
-  <si>
-    <t>RO59 QBHB 45YP PGFQ QLWC Z7GT</t>
-  </si>
-  <si>
-    <t>AD34 7432 1842 GKUB UQPR MDP8</t>
-  </si>
-  <si>
-    <t>BR17 2336 5045 6430 3142 7267 630B Z</t>
-  </si>
-  <si>
     <t>PL91 8895 8031 4931 2445 5326 8909</t>
   </si>
   <si>
@@ -318,6 +171,153 @@
   </si>
   <si>
     <t>igrača modra</t>
+  </si>
+  <si>
+    <t>FR79 2282 6763 09PW 6IWO 96PK Y07</t>
+  </si>
+  <si>
+    <t>FR31 4834 6092 31UZ W7ZT UGFB R22</t>
+  </si>
+  <si>
+    <t>EE68 7340 1352 5566 3731</t>
+  </si>
+  <si>
+    <t>GR11 1018 094X IYFC PGT3 5INY 7IC</t>
+  </si>
+  <si>
+    <t>AZ19 IUST XYBK VDU4 XFZ2 KMY3 1IKE</t>
+  </si>
+  <si>
+    <t>FR62 0841 1230 28O5 GDVJ MDBC L03</t>
+  </si>
+  <si>
+    <t>PK73 OMZO C53E 3IYE SXAD RTFN</t>
+  </si>
+  <si>
+    <t>EE44 8823 9718 1278 6819</t>
+  </si>
+  <si>
+    <t>CR69 6448 2334 9876 1879 8</t>
+  </si>
+  <si>
+    <t>NL09 TLMT 4085 0135 17</t>
+  </si>
+  <si>
+    <t>FR45 5494 2255 49OE YVWD NGW6 Z14</t>
+  </si>
+  <si>
+    <t>HR20 9159 6225 3934 9298 9</t>
+  </si>
+  <si>
+    <t>EE49 7319 9421 4974 1039</t>
+  </si>
+  <si>
+    <t>FR26 5518 8001 92IY JWZX FEJN C44</t>
+  </si>
+  <si>
+    <t>SA51 71XS OWWW 3KEB N83G HPM9</t>
+  </si>
+  <si>
+    <t>FI35 1242 1345 9527 18</t>
+  </si>
+  <si>
+    <t>IT60 Q802 2504 904M WSUP GBFI UA4</t>
+  </si>
+  <si>
+    <t>HU18 3488 8407 0210 9257 0388 5034</t>
+  </si>
+  <si>
+    <t>HR68 1204 4287 4917 3008 3</t>
+  </si>
+  <si>
+    <t>SE80 8624 0816 4622 9352 3647</t>
+  </si>
+  <si>
+    <t>SI96 2089 1193 9003 267</t>
+  </si>
+  <si>
+    <t>SE58 0549 2590 2624 9416 9223</t>
+  </si>
+  <si>
+    <t>FR08 9965 9725 56QB DKF1 0MIN V61</t>
+  </si>
+  <si>
+    <t>FR44 5480 3794 60TT ZIJN KQQ3 F27</t>
+  </si>
+  <si>
+    <t>SA02 473T FNEI JBKI OPR0 VG0F</t>
+  </si>
+  <si>
+    <t>TR93 0116 92B2 WUSO G3LX EHUX PG</t>
+  </si>
+  <si>
+    <t>SA14 085X WT62 45NY J1MD JU14</t>
+  </si>
+  <si>
+    <t>FR55 8004 4030 44EB BN7T BDI1 Q19</t>
+  </si>
+  <si>
+    <t>MR69 1237 3041 8942 8641 5683 215</t>
+  </si>
+  <si>
+    <t>IE57 ZYQA 5080 9339 3722 31</t>
+  </si>
+  <si>
+    <t>MT21 GHVM 2935 6HIR ZVLQ 9ZB4 OPJS 5D6</t>
+  </si>
+  <si>
+    <t>RO21 RAMB 9LQ7 OEPB 5NEI 1MDO</t>
+  </si>
+  <si>
+    <t>MD47 YNEH Z2QJ UHWR UBFB KIBJ</t>
+  </si>
+  <si>
+    <t>FR51 7169 3117 31IQ PRHL TDAT L25</t>
+  </si>
+  <si>
+    <t>FR74 3246 0841 70UY HYFL P81N X77</t>
+  </si>
+  <si>
+    <t>GR48 8581 0775 PIN0 1XSD AMKQ MUE</t>
+  </si>
+  <si>
+    <t>AZ86 KOHM JDOH AEB1 AFRG RAYC DTIH</t>
+  </si>
+  <si>
+    <t>CR49 8336 6285 9676 0875 2</t>
+  </si>
+  <si>
+    <t>GT71 PN5L L1PP ECLG 8YE1 SART MMEG</t>
+  </si>
+  <si>
+    <t>AT12 1475 9491 3950 1051</t>
+  </si>
+  <si>
+    <t>IL83 5273 9999 4201 5858 982</t>
+  </si>
+  <si>
+    <t>ES05 6582 4291 9678 5877 2373</t>
+  </si>
+  <si>
+    <t>FR13 1333 7156 37FM INJW 7JM1 E34</t>
+  </si>
+  <si>
+    <t>RS13 8531 4475 6204 9750 80</t>
+  </si>
+  <si>
+    <t>BE42 3218 6233 1524</t>
+  </si>
+  <si>
+    <t>PS21 KPVI N7BL LJS2 H78H AR5J USXB J</t>
+  </si>
+  <si>
+    <t>MD10 53CZ M45Y GHYV MKKZ ZBMY</t>
+  </si>
+  <si>
+    <t>EE89 8422 6975 3891 9191</t>
+  </si>
+  <si>
+    <t>IT78 X612 8332 086X D7XC 8I04 BNS</t>
   </si>
 </sst>
 </file>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D9432E-CB86-D542-ACDC-ADC3E5EA3E9A}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -703,21 +703,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -725,10 +725,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -736,10 +736,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -769,10 +769,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -879,10 +879,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>7</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>7</v>
@@ -912,10 +912,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>7</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C22">
         <v>7</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C24">
         <v>7</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>7</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C31">
         <v>6</v>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>8</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -1088,10 +1088,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C37">
         <v>8</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C38">
         <v>7</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C40">
         <v>7</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>7</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>7</v>
@@ -1242,10 +1242,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>8</v>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -1286,16 +1286,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1303,13 +1303,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>100000</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1317,13 +1317,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>200000</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1331,13 +1331,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>100000</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1356,10 +1356,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1555,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB253CD-2F29-FA47-9DE4-E4685C4B2BF5}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1566,16 +1566,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1589,7 +1589,7 @@
         <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1603,7 +1603,7 @@
         <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1617,7 +1617,7 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1631,7 +1631,7 @@
         <v>250</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1645,7 +1645,7 @@
         <v>900</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1659,7 +1659,7 @@
         <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1673,7 +1673,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1687,7 +1687,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1701,7 +1701,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1715,7 +1715,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1729,7 +1729,7 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1743,7 +1743,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1757,7 +1757,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1771,7 +1771,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1785,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1799,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1813,7 +1813,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1827,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1841,7 +1841,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1855,7 +1855,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1869,7 +1869,7 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1883,7 +1883,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1897,7 +1897,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>